<commit_message>
Climate Plotter Alpha V1
- Bulk import updated
- partial city view update
- error handling

 TODO: dot sizing, change city view windows to load from external file, Error Handling
</commit_message>
<xml_diff>
--- a/Climate_Fresk_Input_Template.xlsx
+++ b/Climate_Fresk_Input_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Programming\Python\ClimatePlotter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B001258F-94A7-4073-AF3E-C3AAC9D965AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982DB913-DA47-4EAC-9E12-E72B092E0819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24435" yWindow="225" windowWidth="26580" windowHeight="12825" xr2:uid="{44358466-17AC-487B-83DC-D1DD6F554BCF}"/>
+    <workbookView xWindow="-16200" yWindow="-4245" windowWidth="26580" windowHeight="12825" xr2:uid="{44358466-17AC-487B-83DC-D1DD6F554BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>PLZ</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>Datum</t>
-  </si>
-  <si>
-    <t>Uhrzeit</t>
   </si>
 </sst>
 </file>
@@ -229,18 +226,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,220 +557,199 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF58FE2-7165-43D0-9354-A41265EE6F27}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B1" sqref="B1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="30" style="8" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="18" style="8" customWidth="1"/>
+    <col min="6" max="6" width="10" style="8" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="F1" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="G1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{EACEE539-DD13-4C29-8DD0-7D8131606889}">
+  <dataValidations count="2">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{EACEE539-DD13-4C29-8DD0-7D8131606889}">
       <formula1>1067</formula1>
       <formula2>99998</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:I15" xr:uid="{3F5AC59F-7650-44D6-A3A1-87C1F2BA4358}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H15" xr:uid="{3F5AC59F-7650-44D6-A3A1-87C1F2BA4358}">
       <formula1>0</formula1>
       <formula2>2000</formula2>
-    </dataValidation>
-    <dataValidation type="time" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B15" xr:uid="{C0493256-FEC9-4C4C-959A-B615FFCD778B}">
-      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -780,7 +761,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$16</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F15</xm:sqref>
+          <xm:sqref>E2:E15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{92FF6D55-5ED0-4003-AB5C-B60A6191C365}">
           <x14:formula1>

</xml_diff>